<commit_message>
Front end handlers finito
</commit_message>
<xml_diff>
--- a/Frontend Handlers/Frontend Handlers v2.xlsx
+++ b/Frontend Handlers/Frontend Handlers v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nélio\WebApplications\Frontend Handlers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/69b146c70723f936/Faculdade/Mestrado Informática/2º Semestre/Aplicações na Web/WebApplications/Frontend Handlers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A944DB-ABC8-4426-96F6-59E3A645C7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{C4A944DB-ABC8-4426-96F6-59E3A645C7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64FCC8B1-03F3-4E7C-8102-0AC169D91E8F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{7D754FC3-F3DD-437A-AFA7-7EC5AC0A37F6}"/>
+    <workbookView xWindow="2475" yWindow="1350" windowWidth="38700" windowHeight="15345" xr2:uid="{7D754FC3-F3DD-437A-AFA7-7EC5AC0A37F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="87">
   <si>
     <t>Auctions Dashboard</t>
   </si>
@@ -65,9 +65,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>Updated auction data with new bid information</t>
-  </si>
-  <si>
     <t>/auctions/{auctionId}/close</t>
   </si>
   <si>
@@ -113,12 +110,6 @@
     <t>List of search results for items</t>
   </si>
   <si>
-    <t>/recommendations</t>
-  </si>
-  <si>
-    <t>List of recommended auctions/items</t>
-  </si>
-  <si>
     <t>Create Auction</t>
   </si>
   <si>
@@ -233,34 +224,82 @@
     <t>Analytics JSON</t>
   </si>
   <si>
-    <t>Aplicações na Web - Back-End Handlers
+    <t>/payments/{payment_id}</t>
+  </si>
+  <si>
+    <t>/auctions/{auctionId}/payments</t>
+  </si>
+  <si>
+    <t>Auctions</t>
+  </si>
+  <si>
+    <t>/users/{userId}/Auctions</t>
+  </si>
+  <si>
+    <t>/users/{userId}/auctions</t>
+  </si>
+  <si>
+    <t>Aplicações na Web - Front-End Handlers
 Grupo 30:
 Luís Ferreirinha Nº51127 
 Nélio Pereira Nº60550</t>
   </si>
   <si>
-    <t>/auctions/{auctionId}/</t>
-  </si>
-  <si>
-    <t>Payment</t>
-  </si>
-  <si>
-    <t>/payments/{payment_id}</t>
-  </si>
-  <si>
-    <t>/auctions/{auctionId}/payments</t>
-  </si>
-  <si>
-    <t>Payment Service</t>
-  </si>
-  <si>
-    <t>Auctions</t>
-  </si>
-  <si>
-    <t>/users/{userId}/Auctions</t>
-  </si>
-  <si>
-    <t>/users/{userId}/auctions</t>
+    <t>/auctions</t>
+  </si>
+  <si>
+    <t>/users/{userId}/recommendations/items</t>
+  </si>
+  <si>
+    <t>List of recommended items</t>
+  </si>
+  <si>
+    <t>Subscribe to auction</t>
+  </si>
+  <si>
+    <t>Unsubscribe from auction</t>
+  </si>
+  <si>
+    <t>Display Notifications</t>
+  </si>
+  <si>
+    <t>View Payment</t>
+  </si>
+  <si>
+    <t>Perform Payment</t>
+  </si>
+  <si>
+    <t>/auctions/{auctionId}/notifications</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>/auctions/{auctionId}/notifications/{userId}</t>
+  </si>
+  <si>
+    <t>/users/{userId}/notifications</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>Notifications JSON</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>Track a Shipping order</t>
+  </si>
+  <si>
+    <t>/items/{itemId}/shipping/{shippingOrderId}/track</t>
+  </si>
+  <si>
+    <t>Place bid</t>
+  </si>
+  <si>
+    <t>/auctions/{auctionId}/bids</t>
   </si>
 </sst>
 </file>
@@ -419,25 +458,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -755,10 +794,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0622C2D8-0123-4045-B8B7-92293AA405F3}">
-  <dimension ref="C2:H34"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="C2:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,22 +814,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="C2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
@@ -798,21 +840,21 @@
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -820,55 +862,55 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="12"/>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="12"/>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="30" x14ac:dyDescent="0.25">
@@ -880,18 +922,18 @@
         <v>1</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
@@ -900,13 +942,13 @@
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
@@ -924,31 +966,31 @@
         <v>2</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="12"/>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="12"/>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>7</v>
@@ -957,401 +999,491 @@
         <v>5</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="12"/>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>66</v>
+      <c r="F14" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" s="12"/>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="12"/>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="12"/>
       <c r="D18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C19" s="12"/>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="12"/>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="12"/>
       <c r="D21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="G22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="12"/>
       <c r="D23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="12"/>
       <c r="D24" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>25</v>
+      <c r="F24" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C25" s="12"/>
+      <c r="D25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="14"/>
-      <c r="D26" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>28</v>
+      <c r="F26" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="C27" s="16"/>
       <c r="D27" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="12"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D28" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C29" s="12"/>
       <c r="D29" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="12"/>
+      <c r="D30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" s="12"/>
+      <c r="D31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="14"/>
-      <c r="D31" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>35</v>
+      <c r="F31" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="16" t="s">
-        <v>70</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>69</v>
+        <v>1</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="16"/>
       <c r="D33" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="15"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="11"/>
+      <c r="D35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C37" s="11"/>
+      <c r="D37" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="11"/>
+      <c r="D38" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="C2:H3"/>
     <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C34:C35"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="C10:C16"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:H3"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="C25:C26"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="86" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>